<commit_message>
uppfaert skv. abendingum kennara
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t xml:space="preserve">Team:</t>
   </si>
@@ -58,9 +58,6 @@
     <t xml:space="preserve">3 hrs</t>
   </si>
   <si>
-    <t xml:space="preserve">…</t>
-  </si>
-  <si>
     <t xml:space="preserve">Filter tours</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">Set availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel-based pickup</t>
   </si>
 </sst>
 </file>
@@ -245,13 +245,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.71"/>
@@ -295,7 +295,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>1</v>
@@ -304,33 +304,27 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -341,7 +335,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>3</v>
@@ -352,98 +346,98 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
@@ -454,53 +448,58 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>10</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>11</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>12</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>